<commit_message>
Secret santa app added
</commit_message>
<xml_diff>
--- a/Python Demos/1. Introduction of Python/Random_Name_Generator/helper/Data.xlsx
+++ b/Python Demos/1. Introduction of Python/Random_Name_Generator/helper/Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Python\Python-Practice\Python Demos\1. Introduction of Python\Random_Name_Generator\helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Python\Python-Practice\Python Demos\1. Introduction of Python\Random_Name_Generator\helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04AA3C7-64B0-436A-B305-0A304A6A6365}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004259AD-D93C-46B0-9C7F-B5E1BD0DDE41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A6755C9-5963-49C2-A8E4-724C118B154C}"/>
   </bookViews>
   <sheets>
-    <sheet name="FCA_CI" sheetId="1" r:id="rId1"/>
+    <sheet name="Team_Name" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -39,110 +40,32 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Hobby</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
-    <t>H1,H2,H3</t>
+    <t>Emp_Id</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>user1@abc.com</t>
   </si>
   <si>
     <t>Address1</t>
   </si>
   <si>
-    <t>sample Note</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>Address2</t>
-  </si>
-  <si>
-    <t>H1,H2,H4</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>Address3</t>
-  </si>
-  <si>
-    <t>H1,H2,H5</t>
-  </si>
-  <si>
-    <t>user4</t>
-  </si>
-  <si>
-    <t>Address4</t>
-  </si>
-  <si>
-    <t>H1,H2,H6</t>
-  </si>
-  <si>
-    <t>user5</t>
-  </si>
-  <si>
-    <t>Address5</t>
-  </si>
-  <si>
-    <t>H1,H2,H7</t>
-  </si>
-  <si>
-    <t>user6</t>
-  </si>
-  <si>
-    <t>Address6</t>
-  </si>
-  <si>
-    <t>H1,H2,H8</t>
-  </si>
-  <si>
-    <t>user7</t>
-  </si>
-  <si>
-    <t>Address7</t>
-  </si>
-  <si>
-    <t>H1,H2,H9</t>
-  </si>
-  <si>
-    <t>user8</t>
-  </si>
-  <si>
-    <t>Address8</t>
-  </si>
-  <si>
-    <t>H1,H2,H10</t>
-  </si>
-  <si>
-    <t>user9</t>
-  </si>
-  <si>
-    <t>Address9</t>
-  </si>
-  <si>
-    <t>H1,H2,H11</t>
-  </si>
-  <si>
-    <t>user10</t>
-  </si>
-  <si>
-    <t>Address10</t>
-  </si>
-  <si>
-    <t>H1,H2,H12</t>
+    <t>Sample Note</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +75,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -174,13 +105,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -493,176 +427,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED6B9EB-878B-49A5-AF93-7089AACC16B3}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{87FC5667-3C71-4409-A3EA-482E71605A18}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A86D4A2-1534-491A-9C21-B20713BD5770}">
+  <dimension ref="C1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>